<commit_message>
new fixing post processing
</commit_message>
<xml_diff>
--- a/DataWorkbookRubella.xlsx
+++ b/DataWorkbookRubella.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taahir/Downloads/RubellaNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AB2010-1A2F-C74C-8927-DE2A146DD7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D48973C-AEAC-E441-9340-6A90CF2EA3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="3" xr2:uid="{F270E22A-AF68-0948-A29A-BD37CB605717}"/>
   </bookViews>
@@ -1273,7 +1273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9811A8AF-EDA4-A54D-892C-4381AE7679AA}">
   <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView topLeftCell="A99" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A110" sqref="A110:B110"/>
     </sheetView>
   </sheetViews>
@@ -7319,14 +7319,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A4B445-0F45-AA4E-BB0D-75803854B98D}">
   <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="J92" sqref="J92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" t="s">
         <v>125</v>
       </c>
       <c r="B1" s="8" t="s">

</xml_diff>